<commit_message>
Updated documentation. Renamed some modules.
</commit_message>
<xml_diff>
--- a/nqueens/docs/Vergleich_Anzahl_der_Lösungen_Gruessinger.xlsx
+++ b/nqueens/docs/Vergleich_Anzahl_der_Lösungen_Gruessinger.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Vergleich Anzahl der Lösungen</t>
   </si>
@@ -27,7 +27,10 @@
     <t>Anzahl der Damen</t>
   </si>
   <si>
-    <t>Anzahl der Lösungen</t>
+    <t>Erwartete Anzahl an Lösungen</t>
+  </si>
+  <si>
+    <t>Anzahl meiner Lösungen</t>
   </si>
 </sst>
 </file>
@@ -64,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -103,16 +106,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -124,10 +127,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -136,25 +137,12 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -164,11 +152,65 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -177,16 +219,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -238,9 +284,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Vergleich Anzahl der Lösungen</a:t>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Vergleich der Anzahl der Lösungen</a:t>
             </a:r>
+            <a:endParaRPr lang="de-DE">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -278,25 +329,25 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Anzahl der Lösungen</c:v>
+                  <c:v>Anzahl meiner Lösungen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -334,7 +385,7 @@
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inBase"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -436,12 +487,370 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6A54-42B6-A406-5CA2CAEED77D}"/>
+              <c16:uniqueId val="{00000000-5817-4A13-9654-5C1686D3738B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erwartete Anzahl an Lösungen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5462668816039986E-17"/>
+                  <c:y val="-4.6296296296296294E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-4.1666666666666664E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-4.1666666666666664E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0925337632079971E-17"/>
+                  <c:y val="-5.5555555555555552E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-5.5555555555555552E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-7.8703703703703706E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0185067526415994E-16"/>
+                  <c:y val="-8.3333333333333412E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-7.407407407407407E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-6.018518518518521E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-5817-4A13-9654-5C1686D3738B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$B$5:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$D$5:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2680</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5817-4A13-9654-5C1686D3738B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -449,257 +858,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="516473503"/>
-        <c:axId val="572669743"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$B$4</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Anzahl der Damen</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="de-DE"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="ctr"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst>
-                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="35000"/>
-                                <a:lumOff val="65000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                            <a:round/>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
-                <c:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$B$5:$B$13</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
-                      <c:pt idx="0">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>12</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$B$5:$B$13</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="9"/>
-                      <c:pt idx="0">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>6</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>12</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-6A54-42B6-A406-5CA2CAEED77D}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-          </c:ext>
-        </c:extLst>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="396626600"/>
+        <c:axId val="396631192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="516473503"/>
+        <c:axId val="396626600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Anzahl der Damen</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -737,7 +907,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572669743"/>
+        <c:crossAx val="396631192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -745,7 +915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="572669743"/>
+        <c:axId val="396631192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -765,61 +935,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Anzahl der Lösungen</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -851,7 +966,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="516473503"/>
+        <c:crossAx val="396626600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -863,6 +978,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -941,7 +1087,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1145,23 +1291,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1266,8 +1411,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1399,20 +1544,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1449,26 +1593,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CFB0835-1020-495C-B0DD-7010D37F4B96}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1749,106 +1887,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:J19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="27" x14ac:dyDescent="0.6">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:4" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B5" s="3">
+    <row r="5" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="8">
         <v>2</v>
       </c>
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B6" s="5">
+    <row r="6" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>10</v>
       </c>
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B7" s="5">
+    <row r="7" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>4</v>
       </c>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B8" s="5">
+    <row r="8" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>40</v>
       </c>
+      <c r="D8" s="10">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B9" s="5">
+    <row r="9" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>92</v>
       </c>
+      <c r="D9" s="10">
+        <v>92</v>
+      </c>
     </row>
-    <row r="10" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B10" s="5">
+    <row r="10" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>325</v>
       </c>
+      <c r="D10" s="10">
+        <v>352</v>
+      </c>
     </row>
-    <row r="11" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B11" s="5">
+    <row r="11" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>724</v>
       </c>
+      <c r="D11" s="10">
+        <v>724</v>
+      </c>
     </row>
-    <row r="12" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B12" s="5">
+    <row r="12" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>2680</v>
       </c>
+      <c r="D12" s="10">
+        <v>2680</v>
+      </c>
     </row>
-    <row r="13" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="7">
+    <row r="13" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
         <v>12</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="12">
         <v>14200</v>
       </c>
+      <c r="D13" s="11">
+        <v>14200</v>
+      </c>
+    </row>
+    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="6"/>
+    </row>
+    <row r="18" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>